<commit_message>
finalized inspecting the data
</commit_message>
<xml_diff>
--- a/tables/chosen_transitions.xlsx
+++ b/tables/chosen_transitions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
   <si>
     <t xml:space="preserve">Source</t>
   </si>
@@ -43,6 +43,12 @@
     <t xml:space="preserve">Comments</t>
   </si>
   <si>
+    <t xml:space="preserve">Project-code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PI</t>
+  </si>
+  <si>
     <t xml:space="preserve">G008.67</t>
   </si>
   <si>
@@ -64,6 +70,12 @@
     <t xml:space="preserve">Only one available</t>
   </si>
   <si>
+    <t xml:space="preserve">2017.1.00914.S </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Csengeri, Timea</t>
+  </si>
+  <si>
     <t xml:space="preserve">G351.77</t>
   </si>
   <si>
@@ -79,15 +91,15 @@
     <t xml:space="preserve">ALMA-Imf</t>
   </si>
   <si>
-    <t xml:space="preserve">There are more likely regions but I chose the ones that are elongated and do not overlap a lot</t>
-  </si>
-  <si>
     <t xml:space="preserve">member.uid___A001_X122_Xc8.CO.source3.image.pbcor_archive_CO32_res0.7.fits</t>
   </si>
   <si>
     <t xml:space="preserve">Chose resolution closest to alma-imf, instead of 3.5’'</t>
   </si>
   <si>
+    <t xml:space="preserve">2013.1.00960.S</t>
+  </si>
+  <si>
     <t xml:space="preserve">member.uid___A001_X13e_Xc0.G351.77-0.54.CO6-5.image.pbcor.fits</t>
   </si>
   <si>
@@ -97,6 +109,12 @@
     <t xml:space="preserve">not detected?</t>
   </si>
   <si>
+    <t xml:space="preserve">2013.1.00260.S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beuther, Henrik</t>
+  </si>
+  <si>
     <t xml:space="preserve">G328.25</t>
   </si>
   <si>
@@ -112,6 +130,9 @@
     <t xml:space="preserve">member.uid___A001_x005F_X133d_X3488._G328.2551-0.5321_A__sci.spw27.cube.I.pbcor_CO32_res0.354.fits</t>
   </si>
   <si>
+    <t xml:space="preserve">2018.1.01679.S </t>
+  </si>
+  <si>
     <t xml:space="preserve">G337.92</t>
   </si>
   <si>
@@ -125,6 +146,30 @@
   </si>
   <si>
     <t xml:space="preserve">member.uid___A001_x005F_X12a2_X225._G337.9154-0.4773__sci.spw27.cube.I.pbcor_archive_CO32_res0.459.fits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longmore, Steven and many others</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G338.93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G338.93_B6_spw5_12M_spw5.JvM.image.pbcor.statcont.contsub.fits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.56 X 0.51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5,6,7, 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">member.uid___A001_x005F_X12a2_X225._G338.9188p0.5494__sci.spw27.cube.I.pbcor_archive_co32_res0.458.fits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5,6,7,11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5,6 not really elongated, 11 not 100% covered</t>
   </si>
 </sst>
 </file>
@@ -158,12 +203,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF7D1D5"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -200,13 +251,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -218,6 +281,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFF7D1D5"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -398,10 +521,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
+      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -409,35 +532,44 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="26.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="31.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="25.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="38.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>2</v>
@@ -446,22 +578,20 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1"/>
       <c r="B3" s="1" t="n">
         <v>3</v>
       </c>
@@ -469,116 +599,132 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>3.334</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" s="0" t="n">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>19</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>0.658</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="0" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>0.067</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C9" s="0" t="n">
+      <c r="A9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="G9" s="0" t="s">
-        <v>28</v>
+      <c r="G9" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>0.354</v>
@@ -586,47 +732,112 @@
       <c r="F10" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="H10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C12" s="0" t="n">
+      <c r="A12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>31</v>
+      <c r="D12" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>18</v>
+        <v>40</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>0.459</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
+        <v>40</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>0.458</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>